<commit_message>
order workflow inspection image files zip and other fixes
</commit_message>
<xml_diff>
--- a/public/client-files/amc.xlsx
+++ b/public/client-files/amc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\boston\public\client-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A4FEC4E-911D-4C96-8373-F18886BA8AE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2AF9734-7F9B-494F-B96A-AEF559F154B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1525" uniqueCount="506">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1524" uniqueCount="505">
   <si>
     <t>AMC</t>
   </si>
@@ -1612,9 +1612,6 @@
   </si>
   <si>
     <t>Golden Appraisal Ltd</t>
-  </si>
-  <si>
-    <t>a@b.com</t>
   </si>
 </sst>
 </file>
@@ -2015,7 +2012,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2068,9 +2065,7 @@
       <c r="D2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>505</v>
-      </c>
+      <c r="E2" s="5"/>
       <c r="H2" s="1" t="s">
         <v>11</v>
       </c>
@@ -8035,7 +8030,6 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E356" r:id="rId1" xr:uid="{3C43D50C-931A-485C-9852-10F5DA150ABF}"/>
-    <hyperlink ref="E2" r:id="rId2" xr:uid="{D9EAB5BD-123B-4106-8AF0-9E1D8469CDC5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>